<commit_message>
AutoCommit_11 сентября 2023 г. 15:08:23_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-322_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2ИСИП-322_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>2ИСИП-322: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>ок</t>
+  </si>
+  <si>
+    <t>Камилецкий</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -196,6 +199,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -500,13 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -627,7 +633,9 @@
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="2">
         <v>5</v>
       </c>
@@ -894,7 +902,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>1</v>
       </c>
@@ -905,6 +913,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33" spans="2:3" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">

</xml_diff>